<commit_message>
add last exp result
</commit_message>
<xml_diff>
--- a/exp_summary.xlsx
+++ b/exp_summary.xlsx
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +240,15 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -669,8 +678,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -997,8 +1009,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L52" sqref="A31:L52"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="L108" sqref="A108:L127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1418,7 +1430,7 @@
         <v>0.51532199999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>59</v>
       </c>
@@ -1456,7 +1468,7 @@
         <v>0.564747</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>61</v>
       </c>
@@ -1494,7 +1506,7 @@
         <v>0.56431900000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>60</v>
       </c>
@@ -1532,7 +1544,7 @@
         <v>0.56344300000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>57</v>
       </c>
@@ -1570,7 +1582,7 @@
         <v>0.56305799999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>55</v>
       </c>
@@ -1608,7 +1620,7 @@
         <v>0.55782699999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>56</v>
       </c>
@@ -1646,7 +1658,7 @@
         <v>0.55545199999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>58</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>0.555141</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>62</v>
       </c>
@@ -1836,7 +1848,7 @@
         <v>0.49708400000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>42</v>
       </c>
@@ -2102,7 +2114,7 @@
         <v>0.46037699999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>22</v>
       </c>
@@ -2140,7 +2152,7 @@
         <v>0.53359699999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>79</v>
       </c>
@@ -2178,7 +2190,7 @@
         <v>0.52381500000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>104</v>
       </c>
@@ -2216,7 +2228,7 @@
         <v>0.52160200000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>86</v>
       </c>
@@ -2254,7 +2266,7 @@
         <v>0.52159199999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>100</v>
       </c>
@@ -2292,7 +2304,7 @@
         <v>0.52129099999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>89</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>0.31670999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>75</v>
       </c>
@@ -2444,7 +2456,7 @@
         <v>0.51853499999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>93</v>
       </c>
@@ -2520,7 +2532,7 @@
         <v>0.31040800000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>97</v>
       </c>
@@ -2558,7 +2570,7 @@
         <v>0.51393699999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>83</v>
       </c>
@@ -2938,7 +2950,7 @@
         <v>0.53744800000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>71</v>
       </c>
@@ -2976,7 +2988,7 @@
         <v>0.49519400000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>170</v>
       </c>
@@ -3014,7 +3026,7 @@
         <v>0.49444700000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>168</v>
       </c>
@@ -3052,7 +3064,7 @@
         <v>0.49150100000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>173</v>
       </c>
@@ -3090,7 +3102,7 @@
         <v>0.49112099999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>162</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>0.48631600000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>158</v>
       </c>
@@ -3204,7 +3216,7 @@
         <v>0.536219</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>165</v>
       </c>
@@ -3356,7 +3368,7 @@
         <v>0.532501</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>154</v>
       </c>
@@ -3394,7 +3406,7 @@
         <v>0.47761999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>149</v>
       </c>
@@ -3546,7 +3558,7 @@
         <v>0.528918</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>176</v>
       </c>
@@ -3584,7 +3596,7 @@
         <v>0.45935599999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>172</v>
       </c>
@@ -3622,7 +3634,7 @@
         <v>0.45521699999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>175</v>
       </c>
@@ -3660,7 +3672,7 @@
         <v>0.450789</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>145</v>
       </c>
@@ -3698,7 +3710,7 @@
         <v>0.44972499999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>169</v>
       </c>
@@ -3736,7 +3748,7 @@
         <v>0.44510100000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>153</v>
       </c>
@@ -3774,7 +3786,7 @@
         <v>0.43732399999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>166</v>
       </c>
@@ -3812,7 +3824,7 @@
         <v>0.43676500000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>163</v>
       </c>
@@ -3850,7 +3862,7 @@
         <v>0.43492399999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>159</v>
       </c>
@@ -3888,7 +3900,7 @@
         <v>0.43205300000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>179</v>
       </c>
@@ -3926,7 +3938,7 @@
         <v>0.42991499999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>147</v>
       </c>
@@ -3964,7 +3976,7 @@
         <v>0.42275299999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>178</v>
       </c>
@@ -4040,7 +4052,7 @@
         <v>0.41252699999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>177</v>
       </c>
@@ -4116,7 +4128,7 @@
         <v>0.39426299999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>174</v>
       </c>
@@ -4154,7 +4166,7 @@
         <v>0.40982099999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>171</v>
       </c>
@@ -4230,7 +4242,7 @@
         <v>0.52541700000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>140</v>
       </c>
@@ -4306,7 +4318,7 @@
         <v>0.516262</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>142</v>
       </c>
@@ -4344,7 +4356,7 @@
         <v>0.39405000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>167</v>
       </c>
@@ -4382,7 +4394,7 @@
         <v>0.393536</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>164</v>
       </c>
@@ -4496,7 +4508,7 @@
         <v>0.374388</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>157</v>
       </c>
@@ -4534,7 +4546,7 @@
         <v>0.36613800000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>151</v>
       </c>
@@ -4610,7 +4622,7 @@
         <v>0.34179100000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>144</v>
       </c>
@@ -5066,7 +5078,7 @@
         <v>0.28769499999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>63</v>
       </c>
@@ -5104,7 +5116,7 @@
         <v>0.286053</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>46</v>
       </c>
@@ -5332,7 +5344,7 @@
         <v>0.50861500000000004</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>43</v>
       </c>
@@ -5446,7 +5458,7 @@
         <v>0.230769</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>34</v>
       </c>
@@ -5522,7 +5534,7 @@
         <v>0.46820899999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>66</v>
       </c>
@@ -5636,7 +5648,7 @@
         <v>0.194997</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>65</v>
       </c>
@@ -5674,7 +5686,7 @@
         <v>0.18848300000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>30</v>
       </c>
@@ -5712,7 +5724,7 @@
         <v>0.16477700000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>28</v>
       </c>
@@ -5788,7 +5800,7 @@
         <v>0.127495</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>64</v>
       </c>
@@ -6168,7 +6180,7 @@
         <v>8.8190000000000004E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>41</v>
       </c>
@@ -6358,7 +6370,7 @@
         <v>8.4326999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>160</v>
       </c>
@@ -6396,7 +6408,7 @@
         <v>8.1959000000000004E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>40</v>
       </c>
@@ -6434,7 +6446,7 @@
         <v>7.8280000000000002E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>161</v>
       </c>
@@ -6472,7 +6484,7 @@
         <v>7.7451999999999993E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>70</v>
       </c>
@@ -6510,7 +6522,7 @@
         <v>7.6671000000000003E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>50</v>
       </c>
@@ -6548,7 +6560,7 @@
         <v>7.6539999999999997E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>152</v>
       </c>
@@ -6586,7 +6598,7 @@
         <v>7.6385999999999996E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>53</v>
       </c>
@@ -6624,7 +6636,7 @@
         <v>7.5176000000000007E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>156</v>
       </c>
@@ -6662,7 +6674,7 @@
         <v>7.3886999999999994E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>37</v>
       </c>
@@ -6700,7 +6712,7 @@
         <v>7.3663999999999993E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6738,7 +6750,7 @@
         <v>7.2323999999999999E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>155</v>
       </c>
@@ -6776,7 +6788,7 @@
         <v>7.195E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>13</v>
       </c>
@@ -6814,7 +6826,7 @@
         <v>7.1857000000000004E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>54</v>
       </c>
@@ -6852,7 +6864,7 @@
         <v>7.1295999999999998E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>7</v>
       </c>
@@ -6890,7 +6902,7 @@
         <v>7.1012000000000006E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>36</v>
       </c>
@@ -6928,7 +6940,7 @@
         <v>7.0826E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>32</v>
       </c>
@@ -6966,7 +6978,7 @@
         <v>7.0370000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>148</v>
       </c>
@@ -7004,7 +7016,7 @@
         <v>7.0233000000000004E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>38</v>
       </c>
@@ -7042,7 +7054,7 @@
         <v>7.0104E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>69</v>
       </c>
@@ -7080,7 +7092,7 @@
         <v>6.9906999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>68</v>
       </c>
@@ -7118,7 +7130,7 @@
         <v>6.7030999999999993E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>35</v>
       </c>
@@ -7156,7 +7168,7 @@
         <v>6.6923999999999997E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>25</v>
       </c>
@@ -7194,7 +7206,7 @@
         <v>6.6867999999999997E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>16</v>
       </c>
@@ -7232,7 +7244,7 @@
         <v>6.6820000000000004E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>47</v>
       </c>
@@ -7270,7 +7282,7 @@
         <v>6.6752000000000006E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>146</v>
       </c>
@@ -7308,7 +7320,7 @@
         <v>6.6303000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>4</v>
       </c>
@@ -7346,7 +7358,7 @@
         <v>6.6125000000000003E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>49</v>
       </c>
@@ -7384,7 +7396,7 @@
         <v>6.5965999999999997E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>67</v>
       </c>
@@ -7422,7 +7434,7 @@
         <v>6.5950999999999996E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>44</v>
       </c>
@@ -7460,7 +7472,7 @@
         <v>6.4706E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>31</v>
       </c>
@@ -7498,7 +7510,7 @@
         <v>6.4202999999999996E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>1</v>
       </c>
@@ -7536,7 +7548,7 @@
         <v>6.3769999999999993E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>26</v>
       </c>
@@ -7574,7 +7586,7 @@
         <v>6.3710000000000003E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>39</v>
       </c>
@@ -7612,7 +7624,7 @@
         <v>6.3565999999999998E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>48</v>
       </c>
@@ -7650,7 +7662,7 @@
         <v>6.3325000000000006E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>27</v>
       </c>
@@ -7688,7 +7700,7 @@
         <v>6.3198000000000004E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>45</v>
       </c>
@@ -7726,7 +7738,7 @@
         <v>6.2114000000000003E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>143</v>
       </c>
@@ -7764,7 +7776,7 @@
         <v>6.1068999999999998E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>29</v>
       </c>
@@ -7802,7 +7814,7 @@
         <v>6.0996000000000002E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>33</v>
       </c>
@@ -7840,7 +7852,7 @@
         <v>6.0005000000000003E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>141</v>
       </c>
@@ -7887,22 +7899,7 @@
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="bi"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="30"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="256"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="2"/>
+        <filter val="uni"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12105,8 +12102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12408,7 +12405,7 @@
       <c r="K8">
         <v>0.53797099999999998</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>0.53744800000000004</v>
       </c>
     </row>
@@ -12864,7 +12861,7 @@
       <c r="K20">
         <v>0.51513500000000001</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>0.51553300000000002</v>
       </c>
     </row>
@@ -13016,7 +13013,7 @@
       <c r="K24">
         <v>0.52310100000000004</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <v>0.52381500000000003</v>
       </c>
     </row>
@@ -13510,7 +13507,7 @@
       <c r="K37">
         <v>0.56213500000000005</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="1">
         <v>0.564747</v>
       </c>
     </row>
@@ -13675,5 +13672,6 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>